<commit_message>
Added new inputs and FPGA-based velocity measurement for new encoders
</commit_message>
<xml_diff>
--- a/Documentation/Pin Assignments.xlsx
+++ b/Documentation/Pin Assignments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="80">
   <si>
     <t>Connector</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>P5</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>5V+ rail for encoders</t>
+  </si>
+  <si>
+    <t>Ground Rail for encoders</t>
   </si>
 </sst>
 </file>
@@ -337,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -346,6 +355,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1770,13 +1785,403 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+    <row r="72" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="4">
+        <v>50</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2">
+        <v>48</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2">
+        <v>45</v>
+      </c>
+      <c r="C75" s="2">
+        <v>9</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2">
+        <v>9</v>
+      </c>
+      <c r="C76" s="2">
+        <v>7</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2">
+        <v>11</v>
+      </c>
+      <c r="C77" s="2">
+        <v>3</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2">
+        <v>13</v>
+      </c>
+      <c r="C78" s="2">
+        <v>3</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2">
+        <v>15</v>
+      </c>
+      <c r="C79" s="2">
+        <v>3</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2">
+        <v>17</v>
+      </c>
+      <c r="C80" s="2">
+        <v>3</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2">
+        <v>19</v>
+      </c>
+      <c r="C81" s="2">
+        <v>3</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2">
+        <v>21</v>
+      </c>
+      <c r="C82" s="2">
+        <v>3</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2">
+        <v>23</v>
+      </c>
+      <c r="C83" s="2">
+        <v>3</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2">
+        <v>25</v>
+      </c>
+      <c r="C84" s="2">
+        <v>3</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2">
+        <v>27</v>
+      </c>
+      <c r="C85" s="2">
+        <v>3</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2">
+        <v>29</v>
+      </c>
+      <c r="C86" s="2">
+        <v>3</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86" s="4"/>
+      <c r="F86" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2">
+        <v>31</v>
+      </c>
+      <c r="C87" s="2">
+        <v>4</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2">
+        <v>33</v>
+      </c>
+      <c r="C88" s="2">
+        <v>4</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2">
+        <v>35</v>
+      </c>
+      <c r="C89" s="2">
+        <v>4</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2">
+        <v>37</v>
+      </c>
+      <c r="C90" s="2">
+        <v>4</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2">
+        <v>39</v>
+      </c>
+      <c r="C91" s="2">
+        <v>4</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2">
+        <v>41</v>
+      </c>
+      <c r="C92" s="2">
+        <v>4</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2">
+        <v>43</v>
+      </c>
+      <c r="C93" s="2">
+        <v>4</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2">
+        <v>45</v>
+      </c>
+      <c r="C94" s="2">
+        <v>4</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2">
+        <v>47</v>
+      </c>
+      <c r="C95" s="2">
+        <v>4</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A96" s="6"/>
+      <c r="B96" s="6">
+        <v>49</v>
+      </c>
+      <c r="C96" s="6">
+        <v>4</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Verified proper operation, fixed two bugs with new encoders.
</commit_message>
<xml_diff>
--- a/Documentation/Pin Assignments.xlsx
+++ b/Documentation/Pin Assignments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="84">
   <si>
     <t>Connector</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>Ground Rail for encoders</t>
+  </si>
+  <si>
+    <t>Gearbox Encoder 4</t>
+  </si>
+  <si>
+    <t>Gearbox Encoder 3</t>
+  </si>
+  <si>
+    <t>Gearbox Encoder 2</t>
+  </si>
+  <si>
+    <t>Gearbox Encoder 1</t>
   </si>
 </sst>
 </file>
@@ -655,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1797,36 +1809,32 @@
       <c r="A73" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="4">
-        <v>50</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F73" s="4" t="s">
+      <c r="B73" s="2">
+        <v>3</v>
+      </c>
+      <c r="C73" s="2">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2"/>
       <c r="B74" s="2">
-        <v>48</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="C74" s="2">
+        <v>7</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E74" s="2"/>
       <c r="F74" s="2" t="s">
         <v>29</v>
       </c>
@@ -1834,13 +1842,13 @@
     <row r="75" spans="1:6">
       <c r="A75" s="2"/>
       <c r="B75" s="2">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C75" s="2">
-        <v>9</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
@@ -1856,7 +1864,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
@@ -1869,7 +1877,7 @@
         <v>11</v>
       </c>
       <c r="C77" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>16</v>
@@ -1885,7 +1893,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>7</v>
@@ -1901,7 +1909,7 @@
         <v>15</v>
       </c>
       <c r="C79" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>8</v>
@@ -1917,7 +1925,7 @@
         <v>17</v>
       </c>
       <c r="C80" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>9</v>
@@ -1933,7 +1941,7 @@
         <v>19</v>
       </c>
       <c r="C81" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>10</v>
@@ -1949,7 +1957,7 @@
         <v>21</v>
       </c>
       <c r="C82" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>11</v>
@@ -1965,7 +1973,7 @@
         <v>23</v>
       </c>
       <c r="C83" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>12</v>
@@ -1981,7 +1989,7 @@
         <v>25</v>
       </c>
       <c r="C84" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>13</v>
@@ -1997,7 +2005,7 @@
         <v>27</v>
       </c>
       <c r="C85" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>14</v>
@@ -2013,7 +2021,7 @@
         <v>29</v>
       </c>
       <c r="C86" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>15</v>
@@ -2029,12 +2037,14 @@
         <v>31</v>
       </c>
       <c r="C87" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E87" s="2"/>
+      <c r="E87" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F87" s="2" t="s">
         <v>29</v>
       </c>
@@ -2045,7 +2055,7 @@
         <v>33</v>
       </c>
       <c r="C88" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>7</v>
@@ -2061,7 +2071,7 @@
         <v>35</v>
       </c>
       <c r="C89" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>8</v>
@@ -2077,12 +2087,14 @@
         <v>37</v>
       </c>
       <c r="C90" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F90" s="2" t="s">
         <v>29</v>
       </c>
@@ -2093,7 +2105,7 @@
         <v>39</v>
       </c>
       <c r="C91" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>10</v>
@@ -2109,12 +2121,14 @@
         <v>41</v>
       </c>
       <c r="C92" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E92" s="2"/>
+      <c r="E92" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F92" s="2" t="s">
         <v>29</v>
       </c>
@@ -2125,7 +2139,7 @@
         <v>43</v>
       </c>
       <c r="C93" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>12</v>
@@ -2141,12 +2155,14 @@
         <v>45</v>
       </c>
       <c r="C94" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="F94" s="2" t="s">
         <v>29</v>
       </c>
@@ -2157,7 +2173,7 @@
         <v>47</v>
       </c>
       <c r="C95" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>14</v>
@@ -2167,21 +2183,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6">
+    <row r="96" spans="1:6">
+      <c r="A96" s="2"/>
+      <c r="B96" s="4">
         <v>49</v>
       </c>
-      <c r="C96" s="6">
-        <v>4</v>
-      </c>
-      <c r="D96" s="6" t="s">
+      <c r="C96" s="4">
+        <v>9</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="E96" s="4"/>
+      <c r="F96" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="2"/>
+      <c r="B97" s="4">
+        <v>50</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2">
+        <v>48</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>